<commit_message>
ajustando rastreio e valor do driver
</commit_message>
<xml_diff>
--- a/public/model_admin.xlsx
+++ b/public/model_admin.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Task_id</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>tipo</t>
+  </si>
+  <si>
+    <t>valor entrega</t>
   </si>
   <si>
     <t>valor</t>
@@ -165,10 +168,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-ddthh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-ddThh:mm:ss"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,7 +179,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -211,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -219,25 +219,28 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -542,7 +545,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -553,9 +556,9 @@
     <col min="3" max="3" style="8" width="16.862142857142857" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="8" width="16.14785714285714" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="8" width="6.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="5.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="5.2907142857142855" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="8" width="60.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="8.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="8.147857142857141" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="8" width="45.005" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="8" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="8" width="8.719285714285713" customWidth="1" bestFit="1"/>
@@ -565,25 +568,26 @@
     <col min="15" max="15" style="8" width="11.43357142857143" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="7" width="9.862142857142858" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="7" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="8" width="6.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="8" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="8" width="6.005" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="8" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="8" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="8" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="8" width="6.147857142857143" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="9" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="8" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="8" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="8" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="9" width="6.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="9" width="9.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="9" width="6.005" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="9" width="8.005" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="9" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="9" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="9" width="6.147857142857143" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="10" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="10" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="9" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="9" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="9" width="16.14785714285714" customWidth="1" bestFit="1"/>
     <col min="31" max="31" style="8" width="11.005" customWidth="1" bestFit="1"/>
     <col min="32" max="32" style="8" width="4.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="7" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="7" width="5.433571428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,10 +663,10 @@
       <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="AB1" s="2" t="s">
@@ -680,51 +684,54 @@
       <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4">
         <v>29497379</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="H2" s="3"/>
       <c r="I2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N2" s="4">
         <v>0</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P2" s="4">
         <v>-37832218</v>
@@ -732,30 +739,33 @@
       <c r="Q2" s="4">
         <v>-38589607</v>
       </c>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA2" s="6" t="s">
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
+      <c r="AA2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
       <c r="AE2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG2" s="4">
+        <v>48</v>
+      </c>
+      <c r="AG2" s="6">
+        <v>13</v>
+      </c>
+      <c r="AH2" s="4">
         <v>15</v>
       </c>
     </row>

</xml_diff>